<commit_message>
Update OpenCart Database Test Cases.xlsx
</commit_message>
<xml_diff>
--- a/Documents/OpenCart Database Test Cases.xlsx
+++ b/Documents/OpenCart Database Test Cases.xlsx
@@ -49,7 +49,7 @@
     <t>Assignee (Executed By)</t>
   </si>
   <si>
-    <t>DBQ-01</t>
+    <t>TC_DBQ_001</t>
   </si>
   <si>
     <t>Customer</t>
@@ -82,7 +82,7 @@
     <t>Muhammad EmadEl-dien Ali</t>
   </si>
   <si>
-    <t>DBQ-02</t>
+    <t>TC_DBQ_002</t>
   </si>
   <si>
     <t>Check that password is hashed in the database</t>
@@ -103,7 +103,7 @@
     <t>Password should be hashed (not in plain text)</t>
   </si>
   <si>
-    <t>DBQ-03</t>
+    <t>TC_DBQ_003</t>
   </si>
   <si>
     <t>Verify customer login history recorded correctly</t>
@@ -129,7 +129,7 @@
     <t>Login record should exist with correct timestamps</t>
   </si>
   <si>
-    <t>DBQ-04</t>
+    <t>TC_DBQ_004</t>
   </si>
   <si>
     <t>Verify user details are updated after profile edit</t>
@@ -146,7 +146,7 @@
     <t>Updated first and last name should match input</t>
   </si>
   <si>
-    <t>DBQ-05</t>
+    <t>TC_DBQ_005</t>
   </si>
   <si>
     <t>Verify password reset request creates a new token and delete the previouse one</t>
@@ -159,7 +159,7 @@
 Old requests get deleted when the user requests a new password reset</t>
   </si>
   <si>
-    <t>DBQ-06</t>
+    <t>TC_DBQ_006</t>
   </si>
   <si>
     <t>Product</t>
@@ -180,7 +180,7 @@
     <t>Product record should be found with correct details</t>
   </si>
   <si>
-    <t>DBQ-07</t>
+    <t>TC_DBQ_007</t>
   </si>
   <si>
     <t>Verify product price update is reflected</t>
@@ -198,7 +198,7 @@
     <t>Updated price should match new value</t>
   </si>
   <si>
-    <t>DBQ-08</t>
+    <t>TC_DBQ_008</t>
   </si>
   <si>
     <t>Check product quantity update after order</t>
@@ -213,7 +213,7 @@
     <t>Quantity should be reduced by ordered amount</t>
   </si>
   <si>
-    <t>DBQ-09</t>
+    <t>TC_DBQ_009</t>
   </si>
   <si>
     <t>Verify product status updates correctly when disabled</t>
@@ -231,7 +231,7 @@
     <t>Status should be 0 (inactive)</t>
   </si>
   <si>
-    <t>DBQ-10</t>
+    <t>TC_DBQ_010</t>
   </si>
   <si>
     <t>Orders</t>
@@ -252,7 +252,7 @@
     <t>Order record should exist with correct customer and total</t>
   </si>
   <si>
-    <t>DBQ-11</t>
+    <t>TC_DBQ_011</t>
   </si>
   <si>
     <t>Order</t>
@@ -270,7 +270,7 @@
     <t>Order products should match checkout items</t>
   </si>
   <si>
-    <t>DBQ-12</t>
+    <t>TC_DBQ_012</t>
   </si>
   <si>
     <t>Verify order total values are stored correctly</t>
@@ -282,7 +282,7 @@
     <t>Totals should match frontend displayed values</t>
   </si>
   <si>
-    <t>DBQ-13</t>
+    <t>TC_DBQ_013</t>
   </si>
   <si>
     <t>Cart</t>
@@ -304,7 +304,7 @@
     <t>Cart should contain the product with correct quantity</t>
   </si>
   <si>
-    <t>DBQ-14</t>
+    <t>TC_DBQ_014</t>
   </si>
   <si>
     <t>Verify updating product quantity in cart reflects in DB</t>
@@ -320,7 +320,7 @@
     <t>Quantity should match updated value</t>
   </si>
   <si>
-    <t>DBQ-15</t>
+    <t>TC_DBQ_015</t>
   </si>
   <si>
     <t>Verify removing product from cart deletes record</t>
@@ -332,7 +332,7 @@
     <t>No record should exist after deletion</t>
   </si>
   <si>
-    <t>DBQ-16</t>
+    <t>TC_DBQ_016</t>
   </si>
   <si>
     <t>Payment</t>
@@ -347,7 +347,7 @@
     <t>Payment method should match selected option</t>
   </si>
   <si>
-    <t>DBQ-17</t>
+    <t>TC_DBQ_017</t>
   </si>
   <si>
     <t>Verify successful payment updates order status</t>
@@ -359,7 +359,7 @@
     <t>Order status should indicate successful payment</t>
   </si>
   <si>
-    <t>DBQ-18</t>
+    <t>TC_DBQ_018</t>
   </si>
   <si>
     <t>Wishlist</t>
@@ -380,7 +380,7 @@
     <t>Wishlist record should exist</t>
   </si>
   <si>
-    <t>DBQ-19</t>
+    <t>TC_DBQ_019</t>
   </si>
   <si>
     <t>Verify removing product from wishlist deletes record</t>
@@ -399,7 +399,7 @@
     <t>Record should no longer exist</t>
   </si>
   <si>
-    <t>DBQ-20</t>
+    <t>TC_DBQ_020</t>
   </si>
   <si>
     <t>Reviews</t>
@@ -420,7 +420,7 @@
     <t>Review record should exist with matching author name</t>
   </si>
   <si>
-    <t>DBQ-21</t>
+    <t>TC_DBQ_021</t>
   </si>
   <si>
     <t>Check review approval status</t>
@@ -438,7 +438,7 @@
     <t>Status should reflect approved (1) or unapproved (0)</t>
   </si>
   <si>
-    <t>DBQ-22</t>
+    <t>TC_DBQ_022</t>
   </si>
   <si>
     <t>Coupons</t>
@@ -459,7 +459,7 @@
     <t>Coupon record should appear with correct discount value</t>
   </si>
   <si>
-    <t>DBQ-23</t>
+    <t>TC_DBQ_023</t>
   </si>
   <si>
     <t>Admin</t>
@@ -539,10 +539,10 @@
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="0"/>
@@ -866,7 +866,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="9.57"/>
+    <col customWidth="1" min="1" max="1" width="15.71"/>
     <col customWidth="1" min="2" max="2" width="13.0"/>
     <col customWidth="1" min="3" max="3" width="76.57"/>
     <col customWidth="1" min="4" max="4" width="110.29"/>
@@ -923,783 +923,783 @@
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="3"/>
       <c r="J2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="2"/>
+      <c r="L2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="3"/>
       <c r="J4" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="2"/>
+      <c r="L4" s="3"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="2"/>
+      <c r="L5" s="3"/>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="3"/>
       <c r="J6" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="2"/>
+      <c r="L6" s="3"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>49</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="I7" s="3"/>
       <c r="J7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="2"/>
+      <c r="L7" s="3"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>56</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="3"/>
       <c r="J8" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="L8" s="3"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>55</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="3"/>
       <c r="J9" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L9" s="2"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>66</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="I10" s="3"/>
       <c r="J10" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="2"/>
+      <c r="L10" s="3"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="3"/>
       <c r="J11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L11" s="2"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="3"/>
       <c r="J12" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K12" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L12" s="2"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I13" s="3"/>
       <c r="J13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="2"/>
+      <c r="L13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="I14" s="2"/>
+      <c r="I14" s="3"/>
       <c r="J14" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L14" s="2"/>
+      <c r="L14" s="3"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I15" s="2"/>
+      <c r="I15" s="3"/>
       <c r="J15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L15" s="2"/>
+      <c r="L15" s="3"/>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>90</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I16" s="2"/>
+      <c r="I16" s="3"/>
       <c r="J16" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L16" s="2"/>
+      <c r="L16" s="3"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H17" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I17" s="2"/>
+      <c r="I17" s="3"/>
       <c r="J17" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L17" s="2"/>
+      <c r="L17" s="3"/>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E18" s="2" t="s">
         <v>80</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="H18" s="3" t="s">
+      <c r="H18" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="I18" s="2"/>
+      <c r="I18" s="3"/>
       <c r="J18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="2"/>
+      <c r="L18" s="3"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>73</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="I19" s="2"/>
+      <c r="I19" s="3"/>
       <c r="J19" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="2"/>
+      <c r="L19" s="3"/>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>121</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="I20" s="2"/>
+      <c r="I20" s="3"/>
       <c r="J20" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L20" s="2"/>
+      <c r="L20" s="3"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>128</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="I21" s="2"/>
+      <c r="I21" s="3"/>
       <c r="J21" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L21" s="2"/>
+      <c r="L21" s="3"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="2" t="s">
         <v>134</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="I22" s="2"/>
+      <c r="I22" s="3"/>
       <c r="J22" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L22" s="2"/>
+      <c r="L22" s="3"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D23" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>141</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="H23" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="I23" s="2"/>
+      <c r="I23" s="3"/>
       <c r="J23" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L23" s="2"/>
+      <c r="L23" s="3"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="2" t="s">
         <v>148</v>
       </c>
       <c r="F24" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="I24" s="2"/>
+      <c r="I24" s="3"/>
       <c r="J24" s="5" t="s">
         <v>20</v>
       </c>
       <c r="K24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L24" s="2"/>
+      <c r="L24" s="3"/>
     </row>
     <row r="25" ht="15.75" customHeight="1"/>
     <row r="26" ht="15.75" customHeight="1"/>

</xml_diff>